<commit_message>
Instruction and Summary Updates
</commit_message>
<xml_diff>
--- a/Query Summary.xlsx
+++ b/Query Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Documents\GitHub\DATS-6102-Group-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ADE1A1-CC33-4CC8-A197-9BE38F2F6F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EC3D96-7524-412D-B3D3-021296EB391E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
   <si>
     <t>Query Name</t>
   </si>
@@ -140,9 +140,6 @@
     <t>7_2</t>
   </si>
   <si>
-    <t>description = 'Data Analyst'</t>
-  </si>
-  <si>
     <t>description LIKE '%Data Analyst%'</t>
   </si>
   <si>
@@ -284,17 +281,80 @@
     <t>M20</t>
   </si>
   <si>
-    <t>Need to fill in and update the clause columns.</t>
-  </si>
-  <si>
     <t>Times are averages of the data in the Final_data_after_datacleaning file posted 12/1.</t>
+  </si>
+  <si>
+    <t>description IN ('Data Analyst')</t>
+  </si>
+  <si>
+    <t>find({'description' : 'Data Analyst'})</t>
+  </si>
+  <si>
+    <t>find({'description' : { '$in': ['Data Analyst']}})</t>
+  </si>
+  <si>
+    <t>find({'description': {'$regex': 'Data Analyst'}})</t>
+  </si>
+  <si>
+    <t>find({'title' : 'Data Analyst'})</t>
+  </si>
+  <si>
+    <t>find({'title' : { '$in': ['Data Analyst']}})</t>
+  </si>
+  <si>
+    <t>find({'title' : {'$regex': 'Data Analyst'}})</t>
+  </si>
+  <si>
+    <t>find({'title' : {'$not' : {'$eq':'Data Analyst'}}})</t>
+  </si>
+  <si>
+    <t>find({'title' : {'$not' : {'$regex': 'Data Analyst'}}})</t>
+  </si>
+  <si>
+    <t>find({'$or' : [{'title' : 'Data Analyst'} , {'description' : 'Data Analyst'}]})</t>
+  </si>
+  <si>
+    <t>find({'$or' : [{'title' : {'$regex': 'Data Analyst'}} , {'description' : {'$regex': 'Data Analyst'}}]})</t>
+  </si>
+  <si>
+    <t>find({'$and' : [{'title' : 'Data Analyst'} , {'description' : 'Data Analyst'}]})</t>
+  </si>
+  <si>
+    <t>find({'$and' : [{'title' : {'$regex': 'Data Analyst'}} , {'description' : {'$regex': 'Data Analyst'}}]})</t>
+  </si>
+  <si>
+    <t>find({'title' : {'$regex': 'Data Analyst|software engineer'}})</t>
+  </si>
+  <si>
+    <t>find({'title' : {'$regex': 'Data Analyst.*software engineer'}})</t>
+  </si>
+  <si>
+    <t>find({'$or' : [{'title' : {'$regex': 'Data Analyst'}} , {'title' : {'$regex': 'software engineer'}}]})</t>
+  </si>
+  <si>
+    <t>find({'$and' : [{'title' : {'$regex': 'Data Analyst'}} , {'title' : {'$regex': 'software engineer'}}]})</t>
+  </si>
+  <si>
+    <t>find({'title' : 'Data Analyst'},{'title':1, 'company_name':1, 'location':1 })</t>
+  </si>
+  <si>
+    <t>find({'title' : {'$regex': 'Data Analyst'}},{'title':1, 'company_name':1, 'location':1 })</t>
+  </si>
+  <si>
+    <t>find({'description': {'$regex': 'Job [a-zA-Z ]*[^a-zA-Z][a-zA-Z ]*Data Analyst'}})</t>
+  </si>
+  <si>
+    <t>find({'description': {'$regex': '(Job [a-zA-Z ]*[^a-zA-Z][a-zA-Z ]*(d|D)ata (a|A)nalyst.*(j|J)ob (c|C)lassification[^a-zA-Z].*full.time|(c|C)ompensation:[a-zA-Z ]*(N|n)on[^a-zA-Z ][a-zA-Z ]*$\b(1[0-9])\b[^a-zA-Z ]*([3-9][0-9]))'}})</t>
+  </si>
+  <si>
+    <t>Clause columns from visualization_analysis file posted 12/1.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,15 +362,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,11 +376,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -338,18 +386,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -648,7 +693,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,7 +705,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -669,7 +714,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -678,16 +723,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D2" s="1">
         <v>22.724675933333327</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -695,16 +740,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="D3" s="1">
         <v>21.044109846666668</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -712,10 +757,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1">
         <v>29.279327568333333</v>
@@ -723,7 +768,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
       </c>
       <c r="D5" s="1">
         <v>36.970797753333343</v>
@@ -734,10 +785,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1">
         <v>23.460891973333336</v>
@@ -748,10 +799,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1">
         <v>23.453124883333334</v>
@@ -762,10 +813,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1">
         <v>30.743766759999993</v>
@@ -776,10 +827,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1">
         <v>31.119823911666668</v>
@@ -790,10 +841,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D10" s="1">
         <v>22.704437443333333</v>
@@ -804,10 +855,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="D11" s="1">
         <v>19.471743471666667</v>
@@ -818,10 +869,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1">
         <v>29.404865245</v>
@@ -829,7 +880,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
       </c>
       <c r="D13" s="1">
         <v>39.109692156666668</v>
@@ -840,10 +897,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1">
         <v>22.665880646666665</v>
@@ -854,10 +911,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1">
         <v>22.621980099999998</v>
@@ -868,10 +925,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1">
         <v>30.867638333333336</v>
@@ -882,10 +939,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="1">
         <v>31.042467460000001</v>
@@ -896,10 +953,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1">
         <v>34.500668760000011</v>
@@ -910,10 +967,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="1">
         <v>23.091623596666672</v>
@@ -924,10 +981,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1">
         <v>20.690611479999998</v>
@@ -938,10 +995,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1">
         <v>28.306214440000005</v>
@@ -952,10 +1009,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="1">
         <v>31.908325476666668</v>
@@ -966,10 +1023,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="1">
         <v>27.48776761666667</v>
@@ -980,10 +1037,10 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="1">
         <v>24.721344393333329</v>
@@ -994,10 +1051,10 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="1">
         <v>33.559639051666664</v>
@@ -1008,10 +1065,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="1">
         <v>32.672559061666661</v>
@@ -1022,10 +1079,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="1">
         <v>29.833212189999994</v>
@@ -1036,10 +1093,10 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="1">
         <v>19.625839528333334</v>
@@ -1047,13 +1104,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="1">
         <v>38.506603106666667</v>
@@ -1061,13 +1118,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="1">
         <v>22.785402213333334</v>
@@ -1078,10 +1135,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" s="1">
         <v>37.160904423333328</v>
@@ -1092,10 +1149,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="1">
         <v>37.171188435000005</v>
@@ -1106,10 +1163,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="1">
         <v>39.946136626666664</v>
@@ -1120,10 +1177,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" s="1">
         <v>31.107098283333325</v>
@@ -1134,10 +1191,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" s="1">
         <v>306.37667718333336</v>
@@ -1145,7 +1202,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>83</v>
       </c>
       <c r="D36" s="1">
         <v>0.309</v>
@@ -1153,7 +1213,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="C37" t="s">
+        <v>84</v>
       </c>
       <c r="D37" s="1">
         <v>0.30708333333333326</v>
@@ -1161,7 +1224,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
       </c>
       <c r="D38" s="1">
         <v>2.8828</v>
@@ -1169,7 +1235,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
+        <v>86</v>
       </c>
       <c r="D39" s="1">
         <v>0.26750000000000007</v>
@@ -1177,7 +1246,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="C40" t="s">
+        <v>87</v>
       </c>
       <c r="D40" s="1">
         <v>0.26436666666666664</v>
@@ -1185,7 +1257,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="C41" t="s">
+        <v>88</v>
       </c>
       <c r="D41" s="1">
         <v>0.54503333333333326</v>
@@ -1193,7 +1268,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="C42" t="s">
+        <v>89</v>
       </c>
       <c r="D42" s="1">
         <v>0.29767500000000002</v>
@@ -1201,7 +1279,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="C43" t="s">
+        <v>90</v>
       </c>
       <c r="D43" s="1">
         <v>0.54443333333333344</v>
@@ -1209,7 +1290,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="C44" t="s">
+        <v>91</v>
       </c>
       <c r="D44" s="1">
         <v>0.35269166666666668</v>
@@ -1217,7 +1301,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
       </c>
       <c r="D45" s="1">
         <v>3.0974291666666667</v>
@@ -1225,7 +1312,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="C46" t="s">
+        <v>93</v>
       </c>
       <c r="D46" s="1">
         <v>0.32399999999999995</v>
@@ -1233,7 +1323,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="C47" t="s">
+        <v>94</v>
       </c>
       <c r="D47" s="1">
         <v>3.029358333333334</v>
@@ -1241,7 +1334,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
       </c>
       <c r="D48" s="1">
         <v>0.56751666666666678</v>
@@ -1249,7 +1345,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="C49" t="s">
+        <v>96</v>
       </c>
       <c r="D49" s="1">
         <v>0.52469999999999983</v>
@@ -1257,7 +1356,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="C50" t="s">
+        <v>97</v>
       </c>
       <c r="D50" s="1">
         <v>0.67470833333333324</v>
@@ -1265,7 +1367,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
       </c>
       <c r="D51" s="1">
         <v>0.68023333333333358</v>
@@ -1273,7 +1378,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="C52" t="s">
+        <v>99</v>
       </c>
       <c r="D52" s="1">
         <v>0.2898916666666666</v>
@@ -1281,7 +1389,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="C53" t="s">
+        <v>100</v>
       </c>
       <c r="D53" s="1">
         <v>0.67666666666666642</v>
@@ -1289,7 +1400,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="C54" t="s">
+        <v>101</v>
       </c>
       <c r="D54" s="1">
         <v>3.0075874999999996</v>
@@ -1297,7 +1411,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="C55" t="s">
+        <v>102</v>
       </c>
       <c r="D55" s="1">
         <v>13.247699999999998</v>

</xml_diff>

<commit_message>
Submitted Paper and Slides
</commit_message>
<xml_diff>
--- a/Query Summary.xlsx
+++ b/Query Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Documents\GitHub\DATS-6102-Group-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9777450-28CF-403E-8756-BD7DA5D7D281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA70DF05-BD08-4384-858E-686F9BBB0A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -732,20 +732,20 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="64.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="64.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -765,7 +765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -785,7 +785,7 @@
         <v>20.662443426666702</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -805,7 +805,7 @@
         <v>20.540378903333341</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -825,7 +825,7 @@
         <v>29.20788680499999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -845,7 +845,7 @@
         <v>39.375743815000007</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -868,7 +868,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -888,7 +888,7 @@
         <v>23.090971123333329</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -908,7 +908,7 @@
         <v>30.51067897166666</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -928,7 +928,7 @@
         <v>30.954689761666668</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -948,7 +948,7 @@
         <v>19.918397619999997</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -968,7 +968,7 @@
         <v>19.88578686833333</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -988,7 +988,7 @@
         <v>28.593318384999993</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>57</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>38.598469033333338</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>22.357388346666667</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>22.580527941666674</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>31.121311931666661</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>30.317812180000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>34.906590094999999</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>22.520900973333333</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>19.934012814999999</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>27.408485636666676</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>31.404875131666667</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>27.392774786666671</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>25.00667004333334</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>35.021589534999997</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>34.520205066666662</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>31.099031364999995</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>20.142436789999998</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>30.515239596666671</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>20.24523189833333</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>34.560249853333325</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>34.994813801666666</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>35.371231330000001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>30.660288218333324</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>220.08614465666659</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>0.31256666666666655</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>0.29309999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>3.115533333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>0.28284999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>0.58854999999999991</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>0.30773333333333325</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>0.58326666666666671</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>0.37488333333333324</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>3.2819666666666674</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>0.32880000000000004</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>3.3125000000000013</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>0.60993333333333344</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>73</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>0.56850000000000012</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>0.72016666666666684</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>75</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>0.73366666666666669</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>0.29926666666666668</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>77</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>0.71249999999999991</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>3.2000000000000011</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>79</v>
       </c>

</xml_diff>